<commit_message>
Add predefined archetype aggregator and update docs
</commit_message>
<xml_diff>
--- a/data/archetypes/predefined_archetypes.xlsx
+++ b/data/archetypes/predefined_archetypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Greenbean\Shopper\projects\yummi\data\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B31721-99C7-450A-9378-E1DE91AFC597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42089C87-7319-4345-8CD0-C80F9565CE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8AF1ED3B-5AB5-4E86-A044-410CA3F8AB09}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="14">
   <si>
     <t>None</t>
   </si>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E420AEBC-B9F9-4B69-909E-ED53A7C3D25E}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,9 +489,7 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -500,9 +498,7 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -511,9 +507,7 @@
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -522,9 +516,7 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -533,9 +525,7 @@
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -544,9 +534,7 @@
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -555,9 +543,7 @@
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -566,9 +552,7 @@
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -577,9 +561,7 @@
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -588,9 +570,7 @@
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -599,9 +579,7 @@
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -610,9 +588,7 @@
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -621,9 +597,7 @@
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -632,9 +606,7 @@
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -643,9 +615,7 @@
       <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -654,9 +624,7 @@
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -665,9 +633,7 @@
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -676,9 +642,7 @@
       <c r="B19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -687,9 +651,7 @@
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -698,9 +660,7 @@
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -709,9 +669,7 @@
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -720,9 +678,7 @@
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -731,9 +687,7 @@
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -742,9 +696,7 @@
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -753,9 +705,7 @@
       <c r="B26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -764,9 +714,7 @@
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -775,9 +723,7 @@
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -786,9 +732,7 @@
       <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -797,9 +741,7 @@
       <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -808,9 +750,7 @@
       <c r="B31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">

</xml_diff>